<commit_message>
WIP: saving work on demo notebook
</commit_message>
<xml_diff>
--- a/src/data/poster_problem/3_comp_linear_hydrocarbons.xlsx
+++ b/src/data/poster_problem/3_comp_linear_hydrocarbons.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\kevin\Desktop\sns_modeling\src\data\poster_problem\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{41E56864-269B-4C8E-ABD8-9797425ACBA0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6790E2DE-690E-420A-A631-612C3B654F61}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-24120" yWindow="-2235" windowWidth="24240" windowHeight="13020" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="system" sheetId="1" r:id="rId1"/>
@@ -454,8 +454,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:E2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C2" sqref="C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D3" sqref="D3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -486,7 +486,7 @@
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
-        <v>250</v>
+        <v>400</v>
       </c>
       <c r="B2" s="2">
         <v>1</v>
@@ -499,8 +499,8 @@
         <v>1.5E-3</v>
       </c>
       <c r="E2" s="1">
-        <f>5000/1000000</f>
-        <v>5.0000000000000001E-3</v>
+        <f>990000/1000000</f>
+        <v>0.99</v>
       </c>
     </row>
   </sheetData>
@@ -513,7 +513,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5B4ED9-9AA6-42DD-91B2-CD44C4CD8B29}">
   <dimension ref="A1:H12"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
@@ -562,10 +562,10 @@
         <v>0</v>
       </c>
       <c r="C2" s="2">
-        <v>0.2</v>
+        <v>0.3</v>
       </c>
       <c r="D2" s="2">
-        <v>7</v>
+        <v>12</v>
       </c>
       <c r="E2" s="2">
         <v>877</v>
@@ -588,10 +588,10 @@
         <v>1</v>
       </c>
       <c r="C3" s="2">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="D3" s="2">
-        <v>4</v>
+        <v>3.2</v>
       </c>
       <c r="E3" s="2">
         <v>868</v>
@@ -614,7 +614,7 @@
         <v>2</v>
       </c>
       <c r="C4" s="2">
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="D4" s="2">
         <v>1</v>

</xml_diff>